<commit_message>
updated database to include chemical names
</commit_message>
<xml_diff>
--- a/bmd2Samps/data/ChemicalDescriptions.xlsx
+++ b/bmd2Samps/data/ChemicalDescriptions.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/bmd2Samps/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{3E8F46E8-3A83-400C-A1D4-CB60954EF83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BB69084-0443-4407-B5B9-19F6545ED7CE}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{3E8F46E8-3A83-400C-A1D4-CB60954EF83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95C82067-F2D9-479B-85A9-28903BADBB5F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21135" yWindow="1260" windowWidth="21765" windowHeight="22005" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemical List (589)" sheetId="5" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Chemical List (589)'!$A$1:$GK$1701</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5831" uniqueCount="5134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5868" uniqueCount="5153">
   <si>
     <t>DTXSID</t>
   </si>
@@ -15432,6 +15435,63 @@
   </si>
   <si>
     <t>16766-31-7</t>
+  </si>
+  <si>
+    <t>1-Methylpyrene is a member of pyrenes.</t>
+  </si>
+  <si>
+    <t>1-methylphenanthrene is a member of the class of phenanthrenes that is phenanthrene substituted by a methyl group at position 1. It has a role as a mutagen.</t>
+  </si>
+  <si>
+    <t>Benzo[c]fluorene is a carbotetracyclic compound.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Picene is a hydrocarbon found in the pitchy residue obtained in the distillation of peat tar and of petroleum. </t>
+  </si>
+  <si>
+    <t>Dibenzopyrenes are a group of high molecular weight polycyclic aromatic hydrocarbons with the molecular formula C24H14</t>
+  </si>
+  <si>
+    <t>1,2-Dibromo-3-chloropropane, (dibromochloropropane) better known as DBCP, is the organic compound with the formula BrCH(CH2Br)(CH2Cl). It is a dense colorless liquid although commercial samples often appear amber or even brown. It is the active ingredient in the nematicide Nemagon, also known as Fumazone.</t>
+  </si>
+  <si>
+    <t>1-Naphthylamine is an aromatic amine derived from naphthalene. It can cause bladder cancer (transitional cell carcinoma). It crystallizes in colorless needles which melt at 50 °C. </t>
+  </si>
+  <si>
+    <t>Mitotane, sold under the brand name Lysodren, is a steroidogenesis inhibitor and cytostatic antineoplastic medication which is used in the treatment of adrenocortical carcinoma and Cushing's syndrome.</t>
+  </si>
+  <si>
+    <t>No description</t>
+  </si>
+  <si>
+    <t>2,6-Dichlorophenol is a compound with formula C6H3Cl2OH. It is one of the six isomers of dichlorophenol. It is a colorless solid.</t>
+  </si>
+  <si>
+    <t>2-Nitroaniline is an organic compound with the formula H2NC6H4NO2. It is a derivative of aniline, carrying a nitro functional group in position 2.</t>
+  </si>
+  <si>
+    <t>meta-Cresol, also 3-methylphenol, is an organic compound with the formula CH3C6H4(OH). It is a colourless, viscous liquid that is used as an intermediate in the production of other chemicals</t>
+  </si>
+  <si>
+    <t>3-Nitroaniline, also known as meta-nitroaniline and m-nitroaniline, is a non-volatile stable solid commonly used as a raw material for dyes. </t>
+  </si>
+  <si>
+    <t>4-Aminobiphenyl (4-APB) is an organic compound with the formula C6H5C6H4NH2. It is an amine derivative of biphenyl. It is a colorless solid, although aged samples can appear colored. 4-Aminobiphenyl was commonly used in the past as a rubber antioxidant and an intermediate for dyes.</t>
+  </si>
+  <si>
+    <t>α-Hexachlorocyclohexane (α-HCH) is an organochloride which is one of the isomers of hexachlorocyclohexane (HCH). It is a byproduct of the production of the insecticide lindane (γ-HCH) and it is typically still contained in commercial grade lindane used as insecticide.</t>
+  </si>
+  <si>
+    <t>Animocarb (Matacil) is an organic chemical compound with the molecular formula C11H16N2O2. It has a colorless or white crystal-like appearance and is most commonly used as an insecticide.</t>
+  </si>
+  <si>
+    <t>Captafol is a fungicide. It is used to control almost all fungal diseases of plants except powdery mildews. It is believed to be a human carcinogen, and production for use as a fungicide in the United States stopped in 1987. </t>
+  </si>
+  <si>
+    <t>Carbophenothion also known as Stauffer R 1303 as for the manufacturer, Stauffer Chemical, is an organophosphorus chemical compound. It was used as a pesticide for citrus fruits under the name of Trithion</t>
+  </si>
+  <si>
+    <t>Chlorfenvinphos is the common name of an organophosphorus compound that was widely used as an insecticide and an acaricide. The molecule itself can be described as an enol ester derived from dichloroacetophenone and diethylphosphonic acid.</t>
   </si>
 </sst>
 </file>
@@ -15947,8 +16007,8 @@
   <dimension ref="A1:H1701"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A591" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G603" sqref="G603"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F612" sqref="F612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15958,7 +16018,7 @@
     <col min="3" max="3" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="56.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="103.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -20309,7 +20369,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="165" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>259</v>
       </c>
@@ -20621,7 +20681,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>2563</v>
       </c>
@@ -23455,7 +23515,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="289" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A289" s="2" t="s">
         <v>1673</v>
       </c>
@@ -23637,7 +23697,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="296" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A296" s="2" t="s">
         <v>2700</v>
       </c>
@@ -30813,7 +30873,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="572" spans="1:8" ht="165" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A572" s="2" t="s">
         <v>767</v>
       </c>
@@ -31308,251 +31368,362 @@
       </c>
     </row>
     <row r="591" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F591" s="3" t="s">
+        <v>5134</v>
+      </c>
       <c r="H591" s="13" t="s">
         <v>4023</v>
       </c>
     </row>
     <row r="592" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F592" s="3" t="s">
+        <v>5135</v>
+      </c>
       <c r="H592" s="14" t="s">
         <v>4024</v>
       </c>
     </row>
-    <row r="593" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="593" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F593" s="3" t="s">
+        <v>5136</v>
+      </c>
       <c r="H593" s="13" t="s">
         <v>4025</v>
       </c>
     </row>
-    <row r="594" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="594" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G594" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H594" s="14" t="s">
         <v>4026</v>
       </c>
     </row>
-    <row r="595" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="595" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F595" s="3" t="s">
+        <v>5137</v>
+      </c>
       <c r="H595" s="13" t="s">
         <v>4027</v>
       </c>
     </row>
-    <row r="596" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="596" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G596" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H596" s="14" t="s">
         <v>4028</v>
       </c>
     </row>
-    <row r="597" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="597" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F597" s="3" t="s">
+        <v>5138</v>
+      </c>
       <c r="H597" s="13" t="s">
         <v>4029</v>
       </c>
     </row>
-    <row r="598" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="598" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G598" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H598" s="14" t="s">
         <v>4030</v>
       </c>
     </row>
-    <row r="599" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="599" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F599" s="3" t="s">
+        <v>5139</v>
+      </c>
       <c r="H599" s="13" t="s">
         <v>4031</v>
       </c>
     </row>
-    <row r="600" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="600" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F600" s="3" t="s">
+        <v>5140</v>
+      </c>
       <c r="H600" s="14" t="s">
         <v>4032</v>
       </c>
     </row>
-    <row r="601" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="601" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G601" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H601" s="13" t="s">
         <v>4033</v>
       </c>
     </row>
-    <row r="602" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="602" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G602" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H602" s="14" t="s">
         <v>4034</v>
       </c>
     </row>
-    <row r="603" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="603" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G603" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H603" s="13" t="s">
         <v>4035</v>
       </c>
     </row>
-    <row r="604" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="604" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G604" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H604" s="14" t="s">
         <v>4036</v>
       </c>
     </row>
-    <row r="605" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="605" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G605" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H605" s="13" t="s">
         <v>4037</v>
       </c>
     </row>
-    <row r="606" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="606" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F606" s="3" t="s">
+        <v>5141</v>
+      </c>
       <c r="H606" s="14" t="s">
         <v>4038</v>
       </c>
     </row>
-    <row r="607" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="607" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G607" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H607" s="13" t="s">
         <v>4039</v>
       </c>
     </row>
-    <row r="608" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="608" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F608" s="3" t="s">
+        <v>5143</v>
+      </c>
       <c r="H608" s="14" t="s">
         <v>4040</v>
       </c>
     </row>
-    <row r="609" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="609" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F609" s="3" t="s">
+        <v>5144</v>
+      </c>
       <c r="H609" s="13" t="s">
         <v>4041</v>
       </c>
     </row>
-    <row r="610" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="610" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G610" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H610" s="14" t="s">
         <v>4042</v>
       </c>
     </row>
-    <row r="611" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="611" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G611" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H611" s="13" t="s">
         <v>4043</v>
       </c>
     </row>
-    <row r="612" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="612" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F612" s="3" t="s">
+        <v>5145</v>
+      </c>
       <c r="H612" s="14" t="s">
         <v>4044</v>
       </c>
     </row>
-    <row r="613" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="613" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F613" s="3" t="s">
+        <v>5146</v>
+      </c>
       <c r="H613" s="13" t="s">
         <v>4045</v>
       </c>
     </row>
-    <row r="614" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="614" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F614" s="3" t="s">
+        <v>5147</v>
+      </c>
       <c r="H614" s="14" t="s">
         <v>4046</v>
       </c>
     </row>
-    <row r="615" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="615" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G615" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H615" s="13" t="s">
         <v>4047</v>
       </c>
     </row>
-    <row r="616" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="616" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F616" s="3" t="s">
+        <v>5148</v>
+      </c>
       <c r="H616" s="14" t="s">
         <v>4048</v>
       </c>
     </row>
-    <row r="617" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="617" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G617" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H617" s="13" t="s">
         <v>4049</v>
       </c>
     </row>
-    <row r="618" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="618" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F618" s="3" t="s">
+        <v>5149</v>
+      </c>
       <c r="H618" s="14" t="s">
         <v>4050</v>
       </c>
     </row>
-    <row r="619" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="619" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G619" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H619" s="13" t="s">
         <v>4051</v>
       </c>
     </row>
-    <row r="620" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="620" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G620" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H620" s="14" t="s">
         <v>4052</v>
       </c>
     </row>
-    <row r="621" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="621" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G621" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H621" s="13" t="s">
         <v>4053</v>
       </c>
     </row>
-    <row r="622" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="622" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F622" s="3" t="s">
+        <v>5150</v>
+      </c>
       <c r="H622" s="14" t="s">
         <v>4054</v>
       </c>
     </row>
-    <row r="623" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="623" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F623" s="3" t="s">
+        <v>5151</v>
+      </c>
       <c r="H623" s="13" t="s">
         <v>4055</v>
       </c>
     </row>
-    <row r="624" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="624" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F624" s="3" t="s">
+        <v>5152</v>
+      </c>
       <c r="H624" s="14" t="s">
         <v>4056</v>
       </c>
     </row>
-    <row r="625" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="625" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G625" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H625" s="13" t="s">
         <v>4057</v>
       </c>
     </row>
-    <row r="626" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="626" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G626" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H626" s="14" t="s">
         <v>4058</v>
       </c>
     </row>
-    <row r="627" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="627" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G627" s="1" t="s">
+        <v>5142</v>
+      </c>
       <c r="H627" s="13" t="s">
         <v>4059</v>
       </c>
     </row>
-    <row r="628" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="628" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H628" s="14" t="s">
         <v>4060</v>
       </c>
     </row>
-    <row r="629" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="629" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H629" s="13" t="s">
         <v>4061</v>
       </c>
     </row>
-    <row r="630" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="630" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H630" s="14" t="s">
         <v>4062</v>
       </c>
     </row>
-    <row r="631" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="631" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H631" s="13" t="s">
         <v>4063</v>
       </c>
     </row>
-    <row r="632" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="632" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H632" s="14" t="s">
         <v>4064</v>
       </c>
     </row>
-    <row r="633" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="633" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H633" s="13" t="s">
         <v>4065</v>
       </c>
     </row>
-    <row r="634" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="634" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H634" s="14" t="s">
         <v>4066</v>
       </c>
     </row>
-    <row r="635" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="635" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H635" s="13" t="s">
         <v>4067</v>
       </c>
     </row>
-    <row r="636" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="636" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H636" s="14" t="s">
         <v>4068</v>
       </c>
     </row>
-    <row r="637" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="637" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H637" s="13" t="s">
         <v>4069</v>
       </c>
     </row>
-    <row r="638" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="638" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H638" s="14" t="s">
         <v>4070</v>
       </c>
     </row>
-    <row r="639" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="639" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H639" s="13" t="s">
         <v>4071</v>
       </c>
     </row>
-    <row r="640" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="640" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H640" s="14" t="s">
         <v>4072</v>
       </c>
@@ -36863,6 +37034,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:GK1701" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:GK664">
     <sortCondition ref="E2:E664"/>
   </sortState>

</xml_diff>